<commit_message>
Added a check for the Payroll Input file to print Company Code
</commit_message>
<xml_diff>
--- a/Payroll/COA - FINAL.xlsx
+++ b/Payroll/COA - FINAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vboxuser\Customers\TOI Files\Payroll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorinan.kasilag\Programs\TOI\Payroll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCB851D-9B68-41B6-845D-C32D8FE32E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA8C647-2E64-48DD-AA94-98C3DBF5A13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{51CE3EBE-B6DB-4A3D-A64F-F07747104ED3}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{51CE3EBE-B6DB-4A3D-A64F-F07747104ED3}"/>
   </bookViews>
   <sheets>
     <sheet name="COA - USE THIS(Sheet1)" sheetId="1" r:id="rId1"/>
@@ -634,9 +634,6 @@
     <t>SMO - SR Med Officer</t>
   </si>
   <si>
-    <t>Workers Comp Assessment-Employer Tax</t>
-  </si>
-  <si>
     <t>TEP_Educational Pro_Deduction</t>
   </si>
   <si>
@@ -704,6 +701,9 @@
   </si>
   <si>
     <t>TEP TEP</t>
+  </si>
+  <si>
+    <t>Workers Comp Assessment - Employer Tax</t>
   </si>
 </sst>
 </file>
@@ -1631,31 +1631,31 @@
   <dimension ref="A1:BI214"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B158" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B175" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B188" sqref="B188"/>
+      <selection pane="bottomRight" activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="41.40625" customWidth="1"/>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
+    <col min="3" max="4" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" s="1" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E1" s="3">
         <v>100100</v>
@@ -1829,15 +1829,15 @@
         <v>705600</v>
       </c>
     </row>
-    <row r="2" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E2" s="5">
         <v>52000</v>
@@ -2011,15 +2011,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="3" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E3" s="5">
         <v>52005</v>
@@ -2193,15 +2193,15 @@
         <v>60005</v>
       </c>
     </row>
-    <row r="4" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E4" s="5">
         <v>52000</v>
@@ -2375,15 +2375,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="5" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E5" s="5">
         <v>52000</v>
@@ -2557,15 +2557,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="6" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E6" s="5">
         <v>52000</v>
@@ -2739,15 +2739,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="7" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E7" s="5">
         <v>52000</v>
@@ -2921,15 +2921,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="8" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E8" s="5">
         <v>52000</v>
@@ -3103,15 +3103,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="9" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E9" s="5">
         <v>52000</v>
@@ -3285,15 +3285,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="10" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E10" s="5">
         <v>52000</v>
@@ -3467,15 +3467,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="11" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E11" s="5">
         <v>52000</v>
@@ -3649,15 +3649,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="12" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E12" s="5">
         <v>52100</v>
@@ -3831,15 +3831,15 @@
         <v>60100</v>
       </c>
     </row>
-    <row r="13" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E13" s="5">
         <v>52100</v>
@@ -4013,15 +4013,15 @@
         <v>60100</v>
       </c>
     </row>
-    <row r="14" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E14" s="5">
         <v>52000</v>
@@ -4195,15 +4195,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="15" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E15" s="5">
         <v>52000</v>
@@ -4377,15 +4377,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="16" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E16" s="5">
         <v>52000</v>
@@ -4559,12 +4559,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="17" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E17" s="5">
         <v>53005</v>
@@ -4738,12 +4738,12 @@
         <v>53005</v>
       </c>
     </row>
-    <row r="18" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E18" s="5">
         <v>52000</v>
@@ -4917,12 +4917,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="19" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E19" s="5">
         <v>52000</v>
@@ -5096,12 +5096,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="20" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E20" s="5">
         <v>52000</v>
@@ -5275,15 +5275,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="21" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E21" s="5">
         <v>52005</v>
@@ -5457,12 +5457,12 @@
         <v>60005</v>
       </c>
     </row>
-    <row r="22" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E22" s="5">
         <v>52000</v>
@@ -5636,12 +5636,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="23" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E23" s="5">
         <v>52000</v>
@@ -5815,12 +5815,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="24" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E24" s="5">
         <v>52000</v>
@@ -5994,12 +5994,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="25" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E25" s="5">
         <v>52000</v>
@@ -6173,12 +6173,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="26" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E26" s="5">
         <v>52000</v>
@@ -6352,12 +6352,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="27" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E27" s="5">
         <v>52000</v>
@@ -6531,12 +6531,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="28" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E28" s="5">
         <v>52000</v>
@@ -6710,12 +6710,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="29" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E29" s="5">
         <v>52000</v>
@@ -6889,12 +6889,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="30" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E30" s="5">
         <v>63005</v>
@@ -7068,15 +7068,15 @@
         <v>63005</v>
       </c>
     </row>
-    <row r="31" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E31" s="5">
         <v>23250</v>
@@ -7250,12 +7250,12 @@
         <v>23250</v>
       </c>
     </row>
-    <row r="32" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E32" s="5">
         <v>52000</v>
@@ -7429,12 +7429,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="33" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E33" s="5">
         <v>52000</v>
@@ -7608,12 +7608,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="34" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E34" s="5">
         <v>52000</v>
@@ -7787,12 +7787,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="35" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E35" s="5">
         <v>52000</v>
@@ -7966,12 +7966,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="36" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E36" s="5">
         <v>52000</v>
@@ -8145,15 +8145,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="37" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E37" s="5">
         <v>23200</v>
@@ -8327,12 +8327,12 @@
         <v>23200</v>
       </c>
     </row>
-    <row r="38" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E38" s="5">
         <v>52000</v>
@@ -8506,12 +8506,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="39" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E39" s="5">
         <v>52000</v>
@@ -8685,12 +8685,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="40" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E40" s="5">
         <v>52000</v>
@@ -8864,12 +8864,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="41" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E41" s="5">
         <v>52000</v>
@@ -9043,15 +9043,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="42" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E42" s="5">
         <v>52005</v>
@@ -9225,12 +9225,12 @@
         <v>60005</v>
       </c>
     </row>
-    <row r="43" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E43" s="5">
         <v>52000</v>
@@ -9404,15 +9404,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="44" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E44" s="5">
         <v>23200</v>
@@ -9586,12 +9586,12 @@
         <v>23200</v>
       </c>
     </row>
-    <row r="45" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E45" s="5">
         <v>52000</v>
@@ -9765,15 +9765,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="46" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E46" s="5">
         <v>52000</v>
@@ -9947,12 +9947,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="47" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E47" s="5">
         <v>14900</v>
@@ -10126,15 +10126,15 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="48" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E48" s="5">
         <v>52000</v>
@@ -10308,12 +10308,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="49" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E49" s="5">
         <v>52100</v>
@@ -10487,12 +10487,12 @@
         <v>60100</v>
       </c>
     </row>
-    <row r="50" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E50" s="5">
         <v>52000</v>
@@ -10666,12 +10666,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="51" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E51" s="5">
         <v>52100</v>
@@ -10845,12 +10845,12 @@
         <v>60100</v>
       </c>
     </row>
-    <row r="52" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E52" s="5">
         <v>52000</v>
@@ -11024,15 +11024,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="53" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E53" s="5">
         <v>52900</v>
@@ -11206,15 +11206,15 @@
         <v>60900</v>
       </c>
     </row>
-    <row r="54" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E54" s="5">
         <v>52105</v>
@@ -11388,12 +11388,12 @@
         <v>60105</v>
       </c>
     </row>
-    <row r="55" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E55" s="5">
         <v>52000</v>
@@ -11567,15 +11567,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="56" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E56" s="5">
         <v>52900</v>
@@ -11749,12 +11749,12 @@
         <v>60900</v>
       </c>
     </row>
-    <row r="57" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E57" s="5">
         <v>52000</v>
@@ -11928,12 +11928,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="58" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E58" s="5">
         <v>14999</v>
@@ -12107,12 +12107,12 @@
         <v>14999</v>
       </c>
     </row>
-    <row r="59" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E59" s="5">
         <v>52000</v>
@@ -12286,12 +12286,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="60" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E60" s="5">
         <v>52000</v>
@@ -12465,12 +12465,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="61" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E61" s="5">
         <v>52000</v>
@@ -12644,12 +12644,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="62" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E62" s="5">
         <v>52000</v>
@@ -12823,12 +12823,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="63" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E63" s="5">
         <v>52000</v>
@@ -13002,12 +13002,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="64" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E64" s="5">
         <v>52000</v>
@@ -13181,12 +13181,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="65" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E65" s="5">
         <v>52500</v>
@@ -13360,12 +13360,12 @@
         <v>60400</v>
       </c>
     </row>
-    <row r="66" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A66" t="s">
         <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E66" s="3">
         <v>52000</v>
@@ -13539,12 +13539,12 @@
         <v>61055</v>
       </c>
     </row>
-    <row r="67" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A67" t="s">
         <v>66</v>
       </c>
       <c r="C67" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E67" s="3">
         <v>52000</v>
@@ -13718,12 +13718,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="68" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A68" t="s">
         <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E68" s="3">
         <v>52000</v>
@@ -13897,12 +13897,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="69" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A69" t="s">
         <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E69" s="3">
         <v>52000</v>
@@ -14076,12 +14076,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="70" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A70" t="s">
         <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E70" s="3">
         <v>52000</v>
@@ -14255,12 +14255,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="71" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A71" t="s">
         <v>70</v>
       </c>
       <c r="C71" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E71" s="3">
         <v>52000</v>
@@ -14434,12 +14434,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="72" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E72" s="5">
         <v>23101</v>
@@ -14613,12 +14613,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="73" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E73" s="5">
         <v>23101</v>
@@ -14792,12 +14792,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="74" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A74" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E74" s="5">
         <v>23101</v>
@@ -14971,12 +14971,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="75" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E75" s="5">
         <v>23101</v>
@@ -15150,12 +15150,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="76" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E76" s="5">
         <v>23101</v>
@@ -15329,12 +15329,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="77" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E77" s="5">
         <v>23101</v>
@@ -15508,12 +15508,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="78" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E78" s="5">
         <v>23101</v>
@@ -15687,12 +15687,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="79" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E79" s="5">
         <v>23101</v>
@@ -15866,12 +15866,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="80" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E80" s="5">
         <v>23101</v>
@@ -16045,12 +16045,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="81" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E81" s="5">
         <v>23101</v>
@@ -16224,12 +16224,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="82" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E82" s="5">
         <v>23101</v>
@@ -16403,12 +16403,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="83" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A83" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E83" s="5">
         <v>23101</v>
@@ -16582,12 +16582,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="84" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E84" s="5">
         <v>14034</v>
@@ -16761,12 +16761,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="85" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A85" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E85" s="5">
         <v>14034</v>
@@ -16940,12 +16940,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="86" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E86" s="5">
         <v>14034</v>
@@ -17119,12 +17119,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="87" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E87" s="5">
         <v>23101</v>
@@ -17298,12 +17298,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="88" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A88" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E88" s="5">
         <v>23101</v>
@@ -17477,12 +17477,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="89" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A89" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E89" s="5">
         <v>14900</v>
@@ -17656,12 +17656,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="90" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E90" s="5">
         <v>14900</v>
@@ -17835,12 +17835,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="91" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E91" s="5">
         <v>14900</v>
@@ -18014,12 +18014,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="92" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E92" s="5">
         <v>14900</v>
@@ -18193,12 +18193,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="93" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A93" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E93" s="5">
         <v>14034</v>
@@ -18372,12 +18372,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="94" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E94" s="5">
         <v>23101</v>
@@ -18551,12 +18551,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="95" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E95" s="5">
         <v>14032</v>
@@ -18730,12 +18730,12 @@
         <v>14032</v>
       </c>
     </row>
-    <row r="96" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A96" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E96" s="5">
         <v>23103</v>
@@ -18909,12 +18909,12 @@
         <v>23103</v>
       </c>
     </row>
-    <row r="97" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E97" s="5">
         <v>14032</v>
@@ -19088,12 +19088,12 @@
         <v>14032</v>
       </c>
     </row>
-    <row r="98" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E98" s="5">
         <v>14034</v>
@@ -19267,12 +19267,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="99" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E99" s="5">
         <v>23103</v>
@@ -19446,12 +19446,12 @@
         <v>23103</v>
       </c>
     </row>
-    <row r="100" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E100" s="5">
         <v>23101</v>
@@ -19625,12 +19625,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="101" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E101" s="5">
         <v>23101</v>
@@ -19804,12 +19804,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="102" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A102" s="2" t="s">
         <v>101</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E102" s="5">
         <v>23101</v>
@@ -19983,12 +19983,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="103" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E103" s="5">
         <v>23101</v>
@@ -20162,12 +20162,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="104" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A104" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E104" s="5">
         <v>23101</v>
@@ -20341,12 +20341,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="105" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A105" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E105" s="5">
         <v>23101</v>
@@ -20520,12 +20520,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="106" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E106" s="5">
         <v>23101</v>
@@ -20699,7 +20699,7 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="107" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
@@ -20707,7 +20707,7 @@
         <v>107</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E107" s="5">
         <v>23103</v>
@@ -20881,7 +20881,7 @@
         <v>23103</v>
       </c>
     </row>
-    <row r="108" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
@@ -20889,7 +20889,7 @@
         <v>107</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E108" s="5">
         <v>23103</v>
@@ -21063,7 +21063,7 @@
         <v>23103</v>
       </c>
     </row>
-    <row r="109" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A109" s="2" t="s">
         <v>108</v>
       </c>
@@ -21071,7 +21071,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E109" s="5">
         <v>23103</v>
@@ -21245,12 +21245,12 @@
         <v>23103</v>
       </c>
     </row>
-    <row r="110" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A110" s="2" t="s">
         <v>109</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E110" s="5">
         <v>14034</v>
@@ -21424,7 +21424,7 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="111" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
@@ -21432,7 +21432,7 @@
         <v>107</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E111" s="5">
         <v>23103</v>
@@ -21606,12 +21606,12 @@
         <v>23103</v>
       </c>
     </row>
-    <row r="112" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E112" s="5">
         <v>14035</v>
@@ -21785,12 +21785,12 @@
         <v>14035</v>
       </c>
     </row>
-    <row r="113" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E113" s="5">
         <v>23102</v>
@@ -21964,12 +21964,12 @@
         <v>23102</v>
       </c>
     </row>
-    <row r="114" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A114" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E114" s="5">
         <v>23102</v>
@@ -22143,12 +22143,12 @@
         <v>23102</v>
       </c>
     </row>
-    <row r="115" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A115" s="2" t="s">
         <v>114</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E115" s="5">
         <v>14034</v>
@@ -22322,12 +22322,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="116" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A116" s="2" t="s">
         <v>115</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E116" s="5">
         <v>14035</v>
@@ -22501,12 +22501,12 @@
         <v>14035</v>
       </c>
     </row>
-    <row r="117" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E117" s="5">
         <v>14034</v>
@@ -22680,12 +22680,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="118" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E118" s="5">
         <v>14031</v>
@@ -22859,12 +22859,12 @@
         <v>14031</v>
       </c>
     </row>
-    <row r="119" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A119" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E119" s="5">
         <v>14031</v>
@@ -23038,12 +23038,12 @@
         <v>14031</v>
       </c>
     </row>
-    <row r="120" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A120" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E120" s="5">
         <v>14031</v>
@@ -23217,12 +23217,12 @@
         <v>14031</v>
       </c>
     </row>
-    <row r="121" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A121" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E121" s="5">
         <v>23101</v>
@@ -23396,12 +23396,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="122" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A122" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E122" s="5">
         <v>14900</v>
@@ -23575,12 +23575,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="123" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A123" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E123" s="5">
         <v>23101</v>
@@ -23754,12 +23754,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="124" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A124" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E124" s="5">
         <v>14034</v>
@@ -23933,12 +23933,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="125" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A125" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E125" s="5">
         <v>14035</v>
@@ -24112,12 +24112,12 @@
         <v>14035</v>
       </c>
     </row>
-    <row r="126" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A126" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E126" s="5">
         <v>61055</v>
@@ -24291,7 +24291,7 @@
         <v>61055</v>
       </c>
     </row>
-    <row r="127" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -24300,12 +24300,12 @@
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
     </row>
-    <row r="128" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A128" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E128" s="5">
         <v>23102</v>
@@ -24479,12 +24479,12 @@
         <v>23102</v>
       </c>
     </row>
-    <row r="129" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A129" s="2" t="s">
         <v>128</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E129" s="5">
         <v>14999</v>
@@ -24658,12 +24658,12 @@
         <v>14999</v>
       </c>
     </row>
-    <row r="130" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A130" s="2" t="s">
         <v>129</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E130" s="5">
         <v>63999</v>
@@ -24837,12 +24837,12 @@
         <v>63999</v>
       </c>
     </row>
-    <row r="131" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A131" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E131" s="5">
         <v>14034</v>
@@ -25016,12 +25016,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="132" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A132" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E132" s="5">
         <v>14034</v>
@@ -25195,12 +25195,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="133" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A133" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E133" s="5">
         <v>14034</v>
@@ -25374,12 +25374,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="134" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A134" s="2" t="s">
         <v>133</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E134" s="5">
         <v>14034</v>
@@ -25553,12 +25553,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="135" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A135" s="2" t="s">
         <v>134</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E135" s="5">
         <v>14900</v>
@@ -25732,12 +25732,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="136" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A136" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E136" s="5">
         <v>14900</v>
@@ -25911,12 +25911,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="137" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A137" s="2" t="s">
         <v>136</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E137" s="5">
         <v>23101</v>
@@ -26090,12 +26090,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="138" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A138" s="2" t="s">
         <v>137</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E138" s="5">
         <v>23101</v>
@@ -26269,12 +26269,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="139" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A139" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E139" s="5">
         <v>23101</v>
@@ -26448,12 +26448,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="140" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A140" s="2" t="s">
         <v>139</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E140" s="5">
         <v>23101</v>
@@ -26627,12 +26627,12 @@
         <v>23101</v>
       </c>
     </row>
-    <row r="141" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A141" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E141" s="5">
         <v>14033</v>
@@ -26806,12 +26806,12 @@
         <v>14033</v>
       </c>
     </row>
-    <row r="142" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A142" s="2" t="s">
         <v>141</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E142" s="5">
         <v>14034</v>
@@ -26985,12 +26985,12 @@
         <v>14034</v>
       </c>
     </row>
-    <row r="143" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A143" s="2" t="s">
         <v>142</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E143" s="5">
         <v>14033</v>
@@ -27164,12 +27164,12 @@
         <v>14033</v>
       </c>
     </row>
-    <row r="144" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A144" s="2" t="s">
         <v>162</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D144" s="2">
         <v>14900</v>
@@ -27346,12 +27346,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="145" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A145" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E145" s="5">
         <v>14900</v>
@@ -27525,12 +27525,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="146" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A146" s="2" t="s">
         <v>164</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D146" s="2">
         <v>14900</v>
@@ -27707,12 +27707,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="147" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A147" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E147" s="5">
         <v>14900</v>
@@ -27886,12 +27886,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="148" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A148" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D148" s="2">
         <v>14900</v>
@@ -28068,12 +28068,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="149" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A149" s="2" t="s">
         <v>167</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E149" s="5">
         <v>14900</v>
@@ -28247,12 +28247,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="150" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A150" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D150" s="2">
         <v>14900</v>
@@ -28429,12 +28429,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="151" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A151" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E151" s="5">
         <v>14900</v>
@@ -28608,12 +28608,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="152" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A152" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E152" s="5">
         <v>14900</v>
@@ -28787,12 +28787,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="153" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A153" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D153" s="2">
         <v>14900</v>
@@ -28969,12 +28969,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="154" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A154" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E154" s="5">
         <v>14900</v>
@@ -29148,12 +29148,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="155" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A155" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D155" s="2">
         <v>14900</v>
@@ -29330,12 +29330,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="156" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A156" s="2" t="s">
         <v>174</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E156" s="5">
         <v>14900</v>
@@ -29509,12 +29509,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="157" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A157" s="2" t="s">
         <v>175</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E157" s="5">
         <v>14900</v>
@@ -29688,12 +29688,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="158" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A158" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D158" s="2">
         <v>14900</v>
@@ -29870,12 +29870,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="159" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A159" s="2" t="s">
         <v>177</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E159" s="5">
         <v>14900</v>
@@ -30049,15 +30049,15 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="160" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A160" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D160" s="2">
         <v>14900</v>
@@ -30234,12 +30234,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="161" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A161" s="2" t="s">
         <v>179</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E161" s="5">
         <v>14900</v>
@@ -30413,12 +30413,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="162" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A162" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D162" s="2">
         <v>14900</v>
@@ -30595,15 +30595,15 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="163" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A163" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E163" s="5">
         <v>14900</v>
@@ -30777,15 +30777,15 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="164" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A164" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D164" s="2">
         <v>14900</v>
@@ -30962,12 +30962,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="165" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A165" s="2" t="s">
         <v>183</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E165" s="5">
         <v>14900</v>
@@ -31141,12 +31141,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="166" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A166" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D166" s="2">
         <v>14900</v>
@@ -31323,12 +31323,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="167" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A167" s="2" t="s">
         <v>185</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E167" s="5">
         <v>14900</v>
@@ -31502,12 +31502,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="168" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A168" s="2" t="s">
         <v>186</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D168" s="2">
         <v>14900</v>
@@ -31684,12 +31684,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="169" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A169" s="2" t="s">
         <v>187</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E169" s="5">
         <v>14900</v>
@@ -31863,12 +31863,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="170" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A170" s="2" t="s">
         <v>188</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D170" s="2">
         <v>14900</v>
@@ -32045,12 +32045,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="171" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A171" s="2" t="s">
         <v>189</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E171" s="5">
         <v>14900</v>
@@ -32224,12 +32224,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="172" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A172" s="2" t="s">
         <v>190</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D172" s="2">
         <v>14900</v>
@@ -32406,12 +32406,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="173" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A173" s="2" t="s">
         <v>191</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E173" s="5">
         <v>14900</v>
@@ -32585,12 +32585,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="174" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A174" s="2" t="s">
         <v>192</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D174" s="2">
         <v>14900</v>
@@ -32767,12 +32767,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="175" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A175" s="2" t="s">
         <v>193</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E175" s="5">
         <v>14900</v>
@@ -32946,12 +32946,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="176" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A176" s="2" t="s">
         <v>194</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E176" s="5">
         <v>14900</v>
@@ -33125,12 +33125,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="177" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A177" s="2" t="s">
         <v>195</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E177" s="5">
         <v>60000</v>
@@ -33304,12 +33304,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="178" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A178" s="2" t="s">
         <v>196</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E178" s="5">
         <v>14900</v>
@@ -33483,12 +33483,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="179" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A179" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E179" s="5">
         <v>52106</v>
@@ -33662,12 +33662,12 @@
         <v>60106</v>
       </c>
     </row>
-    <row r="180" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A180" s="2" t="s">
         <v>198</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E180" s="5">
         <v>14900</v>
@@ -33841,12 +33841,12 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="181" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A181" s="2" t="s">
         <v>199</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E181" s="5">
         <v>52106</v>
@@ -34020,12 +34020,12 @@
         <v>60106</v>
       </c>
     </row>
-    <row r="182" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A182" s="2" t="s">
         <v>200</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E182" s="5">
         <v>52000</v>
@@ -34199,12 +34199,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="183" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A183" s="2" t="s">
         <v>201</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E183" s="5">
         <v>52000</v>
@@ -34378,12 +34378,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="184" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A184" s="2" t="s">
         <v>202</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E184" s="5">
         <v>52000</v>
@@ -34557,12 +34557,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="185" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A185" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E185" s="5">
         <v>63999</v>
@@ -34736,12 +34736,12 @@
         <v>63999</v>
       </c>
     </row>
-    <row r="186" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A186" s="2" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D186" s="2">
         <v>14900</v>
@@ -34918,12 +34918,12 @@
         <v>60200</v>
       </c>
     </row>
-    <row r="187" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A187" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E187" s="5"/>
       <c r="F187" s="5"/>
@@ -34983,12 +34983,12 @@
       <c r="BH187" s="5"/>
       <c r="BI187" s="5"/>
     </row>
-    <row r="188" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A188" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E188" s="5">
         <v>52000</v>
@@ -35162,12 +35162,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="189" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A189" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E189" s="5">
         <v>52000</v>
@@ -35341,12 +35341,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="190" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A190" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E190" s="5">
         <v>52000</v>
@@ -35520,12 +35520,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="191" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A191" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E191" s="5">
         <v>53005</v>
@@ -35699,12 +35699,12 @@
         <v>53005</v>
       </c>
     </row>
-    <row r="192" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A192" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E192" s="5">
         <v>52000</v>
@@ -35878,12 +35878,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="193" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A193" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E193" s="5">
         <v>52000</v>
@@ -36057,12 +36057,12 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="194" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A194" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E194" s="5">
         <v>52100</v>
@@ -36236,12 +36236,12 @@
         <v>60100</v>
       </c>
     </row>
-    <row r="195" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A195" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E195" s="5">
         <v>52000</v>
@@ -36415,133 +36415,133 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="196" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A196" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B196" s="6"/>
       <c r="C196" s="8"/>
     </row>
-    <row r="197" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A197" s="7" t="s">
         <v>144</v>
       </c>
       <c r="B197" s="6"/>
       <c r="C197" s="8"/>
     </row>
-    <row r="198" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A198" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B198" s="6"/>
       <c r="C198" s="8"/>
     </row>
-    <row r="199" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A199" s="7" t="s">
         <v>146</v>
       </c>
       <c r="B199" s="6"/>
       <c r="C199" s="8"/>
     </row>
-    <row r="200" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A200" s="7" t="s">
         <v>147</v>
       </c>
       <c r="B200" s="6"/>
       <c r="C200" s="8"/>
     </row>
-    <row r="201" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A201" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B201" s="6"/>
       <c r="C201" s="8"/>
     </row>
-    <row r="202" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A202" s="7" t="s">
         <v>149</v>
       </c>
       <c r="B202" s="6"/>
       <c r="C202" s="8"/>
     </row>
-    <row r="203" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A203" s="7" t="s">
         <v>150</v>
       </c>
       <c r="B203" s="6"/>
       <c r="C203" s="8"/>
     </row>
-    <row r="204" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A204" s="7" t="s">
         <v>151</v>
       </c>
       <c r="B204" s="6"/>
       <c r="C204" s="8"/>
     </row>
-    <row r="205" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A205" s="7" t="s">
         <v>152</v>
       </c>
       <c r="B205" s="6"/>
       <c r="C205" s="8"/>
     </row>
-    <row r="206" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A206" s="7" t="s">
         <v>153</v>
       </c>
       <c r="B206" s="6"/>
       <c r="C206" s="8"/>
     </row>
-    <row r="207" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A207" s="7" t="s">
         <v>154</v>
       </c>
       <c r="B207" s="6"/>
       <c r="C207" s="8"/>
     </row>
-    <row r="208" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:61" x14ac:dyDescent="0.75">
       <c r="A208" s="7" t="s">
         <v>155</v>
       </c>
       <c r="B208" s="6"/>
       <c r="C208" s="8"/>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A209" s="7" t="s">
         <v>156</v>
       </c>
       <c r="B209" s="6"/>
       <c r="C209" s="8"/>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A210" s="7" t="s">
         <v>157</v>
       </c>
       <c r="B210" s="6"/>
       <c r="C210" s="8"/>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A211" s="9" t="s">
         <v>158</v>
       </c>
       <c r="B211" s="6"/>
       <c r="C211" s="8"/>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A212" s="9" t="s">
         <v>159</v>
       </c>
       <c r="B212" s="6"/>
       <c r="C212" s="8"/>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A213" s="7" t="s">
         <v>160</v>
       </c>
       <c r="B213" s="6"/>
       <c r="C213" s="8"/>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A214" s="7" t="s">
         <v>161</v>
       </c>

</xml_diff>

<commit_message>
Update to Home Dept Codes added
</commit_message>
<xml_diff>
--- a/Payroll/COA - FINAL.xlsx
+++ b/Payroll/COA - FINAL.xlsx
@@ -1,24 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorinan.kasilag\Programs\TOI\Payroll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vboxuser\Projects\TOI-Python\Payroll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA8C647-2E64-48DD-AA94-98C3DBF5A13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1449C07-F5A4-4AD0-8CF9-154A4E0C059E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{51CE3EBE-B6DB-4A3D-A64F-F07747104ED3}"/>
+    <workbookView xWindow="15300" yWindow="5220" windowWidth="38700" windowHeight="12735" xr2:uid="{51CE3EBE-B6DB-4A3D-A64F-F07747104ED3}"/>
   </bookViews>
   <sheets>
     <sheet name="COA - USE THIS(Sheet1)" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'COA - USE THIS(Sheet1)'!$A$1:$BI$195</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'COA - USE THIS(Sheet1)'!$A$1:$BJ$214</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -622,9 +636,6 @@
     <t>Medicare Surtax Adjust - Employee Tax</t>
   </si>
   <si>
-    <t>RLR</t>
-  </si>
-  <si>
     <t>1CM - 1CME</t>
   </si>
   <si>
@@ -701,6 +712,9 @@
   </si>
   <si>
     <t>TEP TEP</t>
+  </si>
+  <si>
+    <t>RLR_RLR</t>
   </si>
   <si>
     <t>Workers Comp Assessment - Employer Tax</t>
@@ -1242,7 +1256,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1253,6 +1267,9 @@
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1309,6 +1326,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>30111</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>86083</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E0C7F05-B86C-111A-38A5-6BCBB5232D00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11002911" cy="2562583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>268269</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>143347</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE750440-8FBA-B470-0790-CD58B8FA83FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2857500"/>
+          <a:ext cx="11241069" cy="3381847"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1628,34 +1738,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564C415C-277C-4055-8EB4-768220830CF2}">
-  <dimension ref="A1:BI214"/>
+  <dimension ref="A1:BJ214"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B175" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B168" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.40625" customWidth="1"/>
-    <col min="2" max="2" width="17.1328125" customWidth="1"/>
-    <col min="3" max="4" width="13.26953125" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="55" width="9.140625" customWidth="1"/>
+    <col min="56" max="56" width="14.5703125" customWidth="1"/>
+    <col min="57" max="62" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="1" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:62" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E1" s="3">
         <v>100100</v>
@@ -1810,34 +1923,37 @@
       <c r="BC1" s="1">
         <v>703000</v>
       </c>
-      <c r="BD1" s="1">
+      <c r="BD1" s="10">
+        <v>700355</v>
+      </c>
+      <c r="BE1" s="1">
         <v>704000</v>
       </c>
-      <c r="BE1" s="1">
+      <c r="BF1" s="1">
         <v>704100</v>
       </c>
-      <c r="BF1" s="1">
+      <c r="BG1" s="1">
         <v>704500</v>
       </c>
-      <c r="BG1" s="1">
+      <c r="BH1" s="1">
         <v>705000</v>
       </c>
-      <c r="BH1" s="1">
+      <c r="BI1" s="1">
         <v>705500</v>
       </c>
-      <c r="BI1" s="1">
+      <c r="BJ1" s="1">
         <v>705600</v>
       </c>
     </row>
-    <row r="2" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E2" s="5">
         <v>52000</v>
@@ -2010,16 +2126,19 @@
       <c r="BI2" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ2" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="3" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E3" s="5">
         <v>52005</v>
@@ -2192,16 +2311,19 @@
       <c r="BI3" s="2">
         <v>60005</v>
       </c>
+      <c r="BJ3" s="2">
+        <v>60005</v>
+      </c>
     </row>
-    <row r="4" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E4" s="5">
         <v>52000</v>
@@ -2374,16 +2496,19 @@
       <c r="BI4" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ4" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="5" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E5" s="5">
         <v>52000</v>
@@ -2556,16 +2681,19 @@
       <c r="BI5" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ5" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="6" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E6" s="5">
         <v>52000</v>
@@ -2738,16 +2866,19 @@
       <c r="BI6" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ6" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="7" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E7" s="5">
         <v>52000</v>
@@ -2920,16 +3051,19 @@
       <c r="BI7" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ7" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="8" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E8" s="5">
         <v>52000</v>
@@ -3102,16 +3236,19 @@
       <c r="BI8" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ8" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="9" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E9" s="5">
         <v>52000</v>
@@ -3284,16 +3421,19 @@
       <c r="BI9" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ9" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="10" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E10" s="5">
         <v>52000</v>
@@ -3466,16 +3606,19 @@
       <c r="BI10" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ10" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="11" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E11" s="5">
         <v>52000</v>
@@ -3648,16 +3791,19 @@
       <c r="BI11" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ11" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="12" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E12" s="5">
         <v>52100</v>
@@ -3830,16 +3976,19 @@
       <c r="BI12" s="2">
         <v>60100</v>
       </c>
+      <c r="BJ12" s="2">
+        <v>60100</v>
+      </c>
     </row>
-    <row r="13" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E13" s="5">
         <v>52100</v>
@@ -4012,16 +4161,19 @@
       <c r="BI13" s="2">
         <v>60100</v>
       </c>
+      <c r="BJ13" s="2">
+        <v>60100</v>
+      </c>
     </row>
-    <row r="14" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E14" s="5">
         <v>52000</v>
@@ -4194,16 +4346,19 @@
       <c r="BI14" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ14" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="15" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E15" s="5">
         <v>52000</v>
@@ -4376,16 +4531,19 @@
       <c r="BI15" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ15" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="16" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E16" s="5">
         <v>52000</v>
@@ -4558,13 +4716,16 @@
       <c r="BI16" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ16" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="17" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E17" s="5">
         <v>53005</v>
@@ -4737,13 +4898,16 @@
       <c r="BI17" s="2">
         <v>53005</v>
       </c>
+      <c r="BJ17" s="2">
+        <v>53005</v>
+      </c>
     </row>
-    <row r="18" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E18" s="5">
         <v>52000</v>
@@ -4916,13 +5080,16 @@
       <c r="BI18" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ18" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="19" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E19" s="5">
         <v>52000</v>
@@ -5095,13 +5262,16 @@
       <c r="BI19" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ19" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="20" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E20" s="5">
         <v>52000</v>
@@ -5274,16 +5444,19 @@
       <c r="BI20" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ20" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="21" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E21" s="5">
         <v>52005</v>
@@ -5456,13 +5629,16 @@
       <c r="BI21" s="2">
         <v>60005</v>
       </c>
+      <c r="BJ21" s="2">
+        <v>60005</v>
+      </c>
     </row>
-    <row r="22" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E22" s="5">
         <v>52000</v>
@@ -5635,13 +5811,16 @@
       <c r="BI22" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ22" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="23" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E23" s="5">
         <v>52000</v>
@@ -5814,13 +5993,16 @@
       <c r="BI23" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ23" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="24" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E24" s="5">
         <v>52000</v>
@@ -5993,13 +6175,16 @@
       <c r="BI24" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ24" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="25" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E25" s="5">
         <v>52000</v>
@@ -6172,13 +6357,16 @@
       <c r="BI25" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ25" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="26" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E26" s="5">
         <v>52000</v>
@@ -6351,13 +6539,16 @@
       <c r="BI26" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ26" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="27" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E27" s="5">
         <v>52000</v>
@@ -6530,13 +6721,16 @@
       <c r="BI27" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ27" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="28" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E28" s="5">
         <v>52000</v>
@@ -6709,13 +6903,16 @@
       <c r="BI28" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ28" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="29" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E29" s="5">
         <v>52000</v>
@@ -6888,13 +7085,16 @@
       <c r="BI29" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ29" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="30" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E30" s="5">
         <v>63005</v>
@@ -7067,16 +7267,19 @@
       <c r="BI30" s="2">
         <v>63005</v>
       </c>
+      <c r="BJ30" s="2">
+        <v>63005</v>
+      </c>
     </row>
-    <row r="31" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E31" s="5">
         <v>23250</v>
@@ -7249,13 +7452,16 @@
       <c r="BI31" s="2">
         <v>23250</v>
       </c>
+      <c r="BJ31" s="2">
+        <v>23250</v>
+      </c>
     </row>
-    <row r="32" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E32" s="5">
         <v>52000</v>
@@ -7428,13 +7634,16 @@
       <c r="BI32" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ32" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="33" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E33" s="5">
         <v>52000</v>
@@ -7607,13 +7816,16 @@
       <c r="BI33" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ33" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="34" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E34" s="5">
         <v>52000</v>
@@ -7786,13 +7998,16 @@
       <c r="BI34" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ34" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="35" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E35" s="5">
         <v>52000</v>
@@ -7965,13 +8180,16 @@
       <c r="BI35" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ35" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="36" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E36" s="5">
         <v>52000</v>
@@ -8144,16 +8362,19 @@
       <c r="BI36" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ36" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="37" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E37" s="5">
         <v>23200</v>
@@ -8326,13 +8547,16 @@
       <c r="BI37" s="2">
         <v>23200</v>
       </c>
+      <c r="BJ37" s="2">
+        <v>23200</v>
+      </c>
     </row>
-    <row r="38" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E38" s="5">
         <v>52000</v>
@@ -8505,13 +8729,16 @@
       <c r="BI38" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ38" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="39" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E39" s="5">
         <v>52000</v>
@@ -8684,13 +8911,16 @@
       <c r="BI39" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ39" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="40" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E40" s="5">
         <v>52000</v>
@@ -8863,13 +9093,16 @@
       <c r="BI40" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ40" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="41" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E41" s="5">
         <v>52000</v>
@@ -9042,16 +9275,19 @@
       <c r="BI41" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ41" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="42" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E42" s="5">
         <v>52005</v>
@@ -9224,13 +9460,16 @@
       <c r="BI42" s="2">
         <v>60005</v>
       </c>
+      <c r="BJ42" s="2">
+        <v>60005</v>
+      </c>
     </row>
-    <row r="43" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E43" s="5">
         <v>52000</v>
@@ -9403,16 +9642,19 @@
       <c r="BI43" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ43" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="44" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E44" s="5">
         <v>23200</v>
@@ -9585,13 +9827,16 @@
       <c r="BI44" s="2">
         <v>23200</v>
       </c>
+      <c r="BJ44" s="2">
+        <v>23200</v>
+      </c>
     </row>
-    <row r="45" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E45" s="5">
         <v>52000</v>
@@ -9764,16 +10009,19 @@
       <c r="BI45" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ45" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="46" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E46" s="5">
         <v>52000</v>
@@ -9946,13 +10194,16 @@
       <c r="BI46" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ46" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="47" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E47" s="5">
         <v>14900</v>
@@ -10125,16 +10376,19 @@
       <c r="BI47" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ47" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="48" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E48" s="5">
         <v>52000</v>
@@ -10307,13 +10561,16 @@
       <c r="BI48" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ48" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="49" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E49" s="5">
         <v>52100</v>
@@ -10486,13 +10743,16 @@
       <c r="BI49" s="2">
         <v>60100</v>
       </c>
+      <c r="BJ49" s="2">
+        <v>60100</v>
+      </c>
     </row>
-    <row r="50" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E50" s="5">
         <v>52000</v>
@@ -10665,13 +10925,16 @@
       <c r="BI50" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ50" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="51" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E51" s="5">
         <v>52100</v>
@@ -10844,13 +11107,16 @@
       <c r="BI51" s="2">
         <v>60100</v>
       </c>
+      <c r="BJ51" s="2">
+        <v>60100</v>
+      </c>
     </row>
-    <row r="52" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E52" s="5">
         <v>52000</v>
@@ -11023,16 +11289,19 @@
       <c r="BI52" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ52" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="53" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E53" s="5">
         <v>52900</v>
@@ -11205,16 +11474,19 @@
       <c r="BI53" s="2">
         <v>60900</v>
       </c>
+      <c r="BJ53" s="2">
+        <v>60900</v>
+      </c>
     </row>
-    <row r="54" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E54" s="5">
         <v>52105</v>
@@ -11387,13 +11659,16 @@
       <c r="BI54" s="2">
         <v>60105</v>
       </c>
+      <c r="BJ54" s="2">
+        <v>60105</v>
+      </c>
     </row>
-    <row r="55" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E55" s="5">
         <v>52000</v>
@@ -11566,16 +11841,19 @@
       <c r="BI55" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ55" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="56" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E56" s="5">
         <v>52900</v>
@@ -11748,13 +12026,16 @@
       <c r="BI56" s="2">
         <v>60900</v>
       </c>
+      <c r="BJ56" s="2">
+        <v>60900</v>
+      </c>
     </row>
-    <row r="57" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E57" s="5">
         <v>52000</v>
@@ -11927,13 +12208,16 @@
       <c r="BI57" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ57" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="58" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E58" s="5">
         <v>14999</v>
@@ -12106,13 +12390,16 @@
       <c r="BI58" s="2">
         <v>14999</v>
       </c>
+      <c r="BJ58" s="2">
+        <v>14999</v>
+      </c>
     </row>
-    <row r="59" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E59" s="5">
         <v>52000</v>
@@ -12285,13 +12572,16 @@
       <c r="BI59" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ59" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="60" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E60" s="5">
         <v>52000</v>
@@ -12464,13 +12754,16 @@
       <c r="BI60" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ60" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="61" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E61" s="5">
         <v>52000</v>
@@ -12643,13 +12936,16 @@
       <c r="BI61" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ61" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="62" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E62" s="5">
         <v>52000</v>
@@ -12822,13 +13118,16 @@
       <c r="BI62" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ62" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="63" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E63" s="5">
         <v>52000</v>
@@ -13001,13 +13300,16 @@
       <c r="BI63" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ63" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="64" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E64" s="5">
         <v>52000</v>
@@ -13180,13 +13482,16 @@
       <c r="BI64" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ64" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="65" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E65" s="5">
         <v>52500</v>
@@ -13359,13 +13664,16 @@
       <c r="BI65" s="2">
         <v>60400</v>
       </c>
+      <c r="BJ65" s="2">
+        <v>60400</v>
+      </c>
     </row>
-    <row r="66" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E66" s="3">
         <v>52000</v>
@@ -13538,13 +13846,16 @@
       <c r="BI66">
         <v>61055</v>
       </c>
+      <c r="BJ66">
+        <v>61055</v>
+      </c>
     </row>
-    <row r="67" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
       <c r="C67" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E67" s="3">
         <v>52000</v>
@@ -13717,13 +14028,16 @@
       <c r="BI67">
         <v>60000</v>
       </c>
+      <c r="BJ67">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="68" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E68" s="3">
         <v>52000</v>
@@ -13896,13 +14210,16 @@
       <c r="BI68">
         <v>60000</v>
       </c>
+      <c r="BJ68">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="69" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E69" s="3">
         <v>52000</v>
@@ -14075,13 +14392,16 @@
       <c r="BI69">
         <v>60000</v>
       </c>
+      <c r="BJ69">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="70" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E70" s="3">
         <v>52000</v>
@@ -14254,13 +14574,16 @@
       <c r="BI70">
         <v>60000</v>
       </c>
+      <c r="BJ70">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="71" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
       <c r="C71" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E71" s="3">
         <v>52000</v>
@@ -14433,13 +14756,16 @@
       <c r="BI71">
         <v>60000</v>
       </c>
+      <c r="BJ71">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="72" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E72" s="5">
         <v>23101</v>
@@ -14612,13 +14938,16 @@
       <c r="BI72" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ72" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="73" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E73" s="5">
         <v>23101</v>
@@ -14791,13 +15120,16 @@
       <c r="BI73" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ73" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="74" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E74" s="5">
         <v>23101</v>
@@ -14970,13 +15302,16 @@
       <c r="BI74" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ74" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="75" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E75" s="5">
         <v>23101</v>
@@ -15149,13 +15484,16 @@
       <c r="BI75" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ75" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="76" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E76" s="5">
         <v>23101</v>
@@ -15328,13 +15666,16 @@
       <c r="BI76" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ76" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="77" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E77" s="5">
         <v>23101</v>
@@ -15507,13 +15848,16 @@
       <c r="BI77" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ77" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="78" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E78" s="5">
         <v>23101</v>
@@ -15686,13 +16030,16 @@
       <c r="BI78" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ78" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="79" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E79" s="5">
         <v>23101</v>
@@ -15865,13 +16212,16 @@
       <c r="BI79" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ79" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="80" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E80" s="5">
         <v>23101</v>
@@ -16044,13 +16394,16 @@
       <c r="BI80" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ80" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="81" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E81" s="5">
         <v>23101</v>
@@ -16223,13 +16576,16 @@
       <c r="BI81" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ81" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="82" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E82" s="5">
         <v>23101</v>
@@ -16402,13 +16758,16 @@
       <c r="BI82" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ82" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="83" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E83" s="5">
         <v>23101</v>
@@ -16581,13 +16940,16 @@
       <c r="BI83" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ83" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="84" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E84" s="5">
         <v>14034</v>
@@ -16760,13 +17122,16 @@
       <c r="BI84" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ84" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="85" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E85" s="5">
         <v>14034</v>
@@ -16939,13 +17304,16 @@
       <c r="BI85" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ85" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="86" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E86" s="5">
         <v>14034</v>
@@ -17118,13 +17486,16 @@
       <c r="BI86" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ86" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="87" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E87" s="5">
         <v>23101</v>
@@ -17297,13 +17668,16 @@
       <c r="BI87" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ87" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="88" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E88" s="5">
         <v>23101</v>
@@ -17476,13 +17850,16 @@
       <c r="BI88" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ88" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="89" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E89" s="5">
         <v>14900</v>
@@ -17655,13 +18032,16 @@
       <c r="BI89" s="5">
         <v>14900</v>
       </c>
+      <c r="BJ89" s="5">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="90" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E90" s="5">
         <v>14900</v>
@@ -17834,13 +18214,16 @@
       <c r="BI90" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ90" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="91" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E91" s="5">
         <v>14900</v>
@@ -18013,13 +18396,16 @@
       <c r="BI91" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ91" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="92" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E92" s="5">
         <v>14900</v>
@@ -18192,13 +18578,16 @@
       <c r="BI92" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ92" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="93" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E93" s="5">
         <v>14034</v>
@@ -18371,13 +18760,16 @@
       <c r="BI93" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ93" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="94" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E94" s="5">
         <v>23101</v>
@@ -18550,13 +18942,16 @@
       <c r="BI94" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ94" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="95" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E95" s="5">
         <v>14032</v>
@@ -18729,13 +19124,16 @@
       <c r="BI95" s="2">
         <v>14032</v>
       </c>
+      <c r="BJ95" s="2">
+        <v>14032</v>
+      </c>
     </row>
-    <row r="96" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E96" s="5">
         <v>23103</v>
@@ -18908,13 +19306,16 @@
       <c r="BI96" s="2">
         <v>23103</v>
       </c>
+      <c r="BJ96" s="2">
+        <v>23103</v>
+      </c>
     </row>
-    <row r="97" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E97" s="5">
         <v>14032</v>
@@ -19087,13 +19488,16 @@
       <c r="BI97" s="2">
         <v>14032</v>
       </c>
+      <c r="BJ97" s="2">
+        <v>14032</v>
+      </c>
     </row>
-    <row r="98" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E98" s="5">
         <v>14034</v>
@@ -19266,13 +19670,16 @@
       <c r="BI98" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ98" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="99" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E99" s="5">
         <v>23103</v>
@@ -19445,13 +19852,16 @@
       <c r="BI99" s="2">
         <v>23103</v>
       </c>
+      <c r="BJ99" s="2">
+        <v>23103</v>
+      </c>
     </row>
-    <row r="100" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E100" s="5">
         <v>23101</v>
@@ -19624,13 +20034,16 @@
       <c r="BI100" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ100" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="101" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E101" s="5">
         <v>23101</v>
@@ -19803,13 +20216,16 @@
       <c r="BI101" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ101" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="102" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>101</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E102" s="5">
         <v>23101</v>
@@ -19982,13 +20398,16 @@
       <c r="BI102" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ102" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="103" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E103" s="5">
         <v>23101</v>
@@ -20161,13 +20580,16 @@
       <c r="BI103" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ103" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="104" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E104" s="5">
         <v>23101</v>
@@ -20340,13 +20762,16 @@
       <c r="BI104" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ104" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="105" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E105" s="5">
         <v>23101</v>
@@ -20519,13 +20944,16 @@
       <c r="BI105" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ105" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="106" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E106" s="5">
         <v>23101</v>
@@ -20698,8 +21126,11 @@
       <c r="BI106" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ106" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="107" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
@@ -20707,7 +21138,7 @@
         <v>107</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E107" s="5">
         <v>23103</v>
@@ -20880,8 +21311,11 @@
       <c r="BI107" s="2">
         <v>23103</v>
       </c>
+      <c r="BJ107" s="2">
+        <v>23103</v>
+      </c>
     </row>
-    <row r="108" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
@@ -20889,7 +21323,7 @@
         <v>107</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E108" s="5">
         <v>23103</v>
@@ -21062,8 +21496,11 @@
       <c r="BI108" s="2">
         <v>23103</v>
       </c>
+      <c r="BJ108" s="2">
+        <v>23103</v>
+      </c>
     </row>
-    <row r="109" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>108</v>
       </c>
@@ -21071,7 +21508,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E109" s="5">
         <v>23103</v>
@@ -21244,13 +21681,16 @@
       <c r="BI109" s="2">
         <v>23103</v>
       </c>
+      <c r="BJ109" s="2">
+        <v>23103</v>
+      </c>
     </row>
-    <row r="110" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>109</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E110" s="5">
         <v>14034</v>
@@ -21423,8 +21863,11 @@
       <c r="BI110" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ110" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="111" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
@@ -21432,7 +21875,7 @@
         <v>107</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E111" s="5">
         <v>23103</v>
@@ -21605,13 +22048,16 @@
       <c r="BI111" s="2">
         <v>23103</v>
       </c>
+      <c r="BJ111" s="2">
+        <v>23103</v>
+      </c>
     </row>
-    <row r="112" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E112" s="5">
         <v>14035</v>
@@ -21784,13 +22230,16 @@
       <c r="BI112" s="2">
         <v>14035</v>
       </c>
+      <c r="BJ112" s="2">
+        <v>14035</v>
+      </c>
     </row>
-    <row r="113" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E113" s="5">
         <v>23102</v>
@@ -21963,13 +22412,16 @@
       <c r="BI113" s="2">
         <v>23102</v>
       </c>
+      <c r="BJ113" s="2">
+        <v>23102</v>
+      </c>
     </row>
-    <row r="114" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E114" s="5">
         <v>23102</v>
@@ -22142,13 +22594,16 @@
       <c r="BI114" s="2">
         <v>23102</v>
       </c>
+      <c r="BJ114" s="2">
+        <v>23102</v>
+      </c>
     </row>
-    <row r="115" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>114</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E115" s="5">
         <v>14034</v>
@@ -22321,13 +22776,16 @@
       <c r="BI115" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ115" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="116" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>115</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E116" s="5">
         <v>14035</v>
@@ -22500,13 +22958,16 @@
       <c r="BI116" s="2">
         <v>14035</v>
       </c>
+      <c r="BJ116" s="2">
+        <v>14035</v>
+      </c>
     </row>
-    <row r="117" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E117" s="5">
         <v>14034</v>
@@ -22679,13 +23140,16 @@
       <c r="BI117" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ117" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="118" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E118" s="5">
         <v>14031</v>
@@ -22858,13 +23322,16 @@
       <c r="BI118" s="2">
         <v>14031</v>
       </c>
+      <c r="BJ118" s="2">
+        <v>14031</v>
+      </c>
     </row>
-    <row r="119" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E119" s="5">
         <v>14031</v>
@@ -23037,13 +23504,16 @@
       <c r="BI119" s="2">
         <v>14031</v>
       </c>
+      <c r="BJ119" s="2">
+        <v>14031</v>
+      </c>
     </row>
-    <row r="120" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E120" s="5">
         <v>14031</v>
@@ -23216,13 +23686,16 @@
       <c r="BI120" s="2">
         <v>14031</v>
       </c>
+      <c r="BJ120" s="2">
+        <v>14031</v>
+      </c>
     </row>
-    <row r="121" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E121" s="5">
         <v>23101</v>
@@ -23395,13 +23868,16 @@
       <c r="BI121" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ121" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="122" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E122" s="5">
         <v>14900</v>
@@ -23574,13 +24050,16 @@
       <c r="BI122" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ122" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="123" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E123" s="5">
         <v>23101</v>
@@ -23753,13 +24232,16 @@
       <c r="BI123" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ123" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="124" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E124" s="5">
         <v>14034</v>
@@ -23932,13 +24414,16 @@
       <c r="BI124" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ124" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="125" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E125" s="5">
         <v>14035</v>
@@ -24111,13 +24596,16 @@
       <c r="BI125" s="2">
         <v>14035</v>
       </c>
+      <c r="BJ125" s="2">
+        <v>14035</v>
+      </c>
     </row>
-    <row r="126" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E126" s="5">
         <v>61055</v>
@@ -24290,8 +24778,11 @@
       <c r="BI126" s="2">
         <v>61055</v>
       </c>
+      <c r="BJ126" s="2">
+        <v>61055</v>
+      </c>
     </row>
-    <row r="127" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -24300,12 +24791,12 @@
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
     </row>
-    <row r="128" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E128" s="5">
         <v>23102</v>
@@ -24478,13 +24969,16 @@
       <c r="BI128" s="2">
         <v>23102</v>
       </c>
+      <c r="BJ128" s="2">
+        <v>23102</v>
+      </c>
     </row>
-    <row r="129" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>128</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E129" s="5">
         <v>14999</v>
@@ -24657,13 +25151,16 @@
       <c r="BI129" s="2">
         <v>14999</v>
       </c>
+      <c r="BJ129" s="2">
+        <v>14999</v>
+      </c>
     </row>
-    <row r="130" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>129</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E130" s="5">
         <v>63999</v>
@@ -24836,13 +25333,16 @@
       <c r="BI130" s="4">
         <v>63999</v>
       </c>
+      <c r="BJ130" s="4">
+        <v>63999</v>
+      </c>
     </row>
-    <row r="131" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E131" s="5">
         <v>14034</v>
@@ -25015,13 +25515,16 @@
       <c r="BI131" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ131" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="132" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E132" s="5">
         <v>14034</v>
@@ -25194,13 +25697,16 @@
       <c r="BI132" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ132" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="133" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E133" s="5">
         <v>14034</v>
@@ -25373,13 +25879,16 @@
       <c r="BI133" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ133" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="134" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>133</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E134" s="5">
         <v>14034</v>
@@ -25552,13 +26061,16 @@
       <c r="BI134" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ134" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="135" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>134</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E135" s="5">
         <v>14900</v>
@@ -25731,13 +26243,16 @@
       <c r="BI135" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ135" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="136" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E136" s="5">
         <v>14900</v>
@@ -25910,13 +26425,16 @@
       <c r="BI136" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ136" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="137" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>136</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E137" s="5">
         <v>23101</v>
@@ -26089,13 +26607,16 @@
       <c r="BI137" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ137" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="138" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>137</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E138" s="5">
         <v>23101</v>
@@ -26268,13 +26789,16 @@
       <c r="BI138" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ138" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="139" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E139" s="5">
         <v>23101</v>
@@ -26447,13 +26971,16 @@
       <c r="BI139" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ139" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="140" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>139</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E140" s="5">
         <v>23101</v>
@@ -26626,13 +27153,16 @@
       <c r="BI140" s="2">
         <v>23101</v>
       </c>
+      <c r="BJ140" s="2">
+        <v>23101</v>
+      </c>
     </row>
-    <row r="141" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E141" s="5">
         <v>14033</v>
@@ -26805,13 +27335,16 @@
       <c r="BI141" s="2">
         <v>14033</v>
       </c>
+      <c r="BJ141" s="2">
+        <v>14033</v>
+      </c>
     </row>
-    <row r="142" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>141</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E142" s="5">
         <v>14034</v>
@@ -26984,13 +27517,16 @@
       <c r="BI142" s="2">
         <v>14034</v>
       </c>
+      <c r="BJ142" s="2">
+        <v>14034</v>
+      </c>
     </row>
-    <row r="143" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>142</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E143" s="5">
         <v>14033</v>
@@ -27163,13 +27699,16 @@
       <c r="BI143" s="2">
         <v>14033</v>
       </c>
+      <c r="BJ143" s="2">
+        <v>14033</v>
+      </c>
     </row>
-    <row r="144" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>162</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D144" s="2">
         <v>14900</v>
@@ -27345,13 +27884,16 @@
       <c r="BI144" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ144" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="145" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E145" s="5">
         <v>14900</v>
@@ -27524,13 +28066,16 @@
       <c r="BI145" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ145" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="146" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>164</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D146" s="2">
         <v>14900</v>
@@ -27706,13 +28251,16 @@
       <c r="BI146" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ146" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="147" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E147" s="5">
         <v>14900</v>
@@ -27885,13 +28433,16 @@
       <c r="BI147" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ147" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="148" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D148" s="2">
         <v>14900</v>
@@ -28067,13 +28618,16 @@
       <c r="BI148" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ148" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="149" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>167</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E149" s="5">
         <v>14900</v>
@@ -28246,13 +28800,16 @@
       <c r="BI149" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ149" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="150" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D150" s="2">
         <v>14900</v>
@@ -28428,13 +28985,16 @@
       <c r="BI150" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ150" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="151" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E151" s="5">
         <v>14900</v>
@@ -28607,13 +29167,16 @@
       <c r="BI151" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ151" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="152" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E152" s="5">
         <v>14900</v>
@@ -28786,13 +29349,16 @@
       <c r="BI152" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ152" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="153" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D153" s="2">
         <v>14900</v>
@@ -28968,13 +29534,16 @@
       <c r="BI153" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ153" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="154" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E154" s="5">
         <v>14900</v>
@@ -29147,13 +29716,16 @@
       <c r="BI154" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ154" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="155" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D155" s="2">
         <v>14900</v>
@@ -29329,13 +29901,16 @@
       <c r="BI155" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ155" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="156" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>174</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E156" s="5">
         <v>14900</v>
@@ -29508,13 +30083,16 @@
       <c r="BI156" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ156" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="157" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>175</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E157" s="5">
         <v>14900</v>
@@ -29687,13 +30265,16 @@
       <c r="BI157" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ157" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="158" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D158" s="2">
         <v>14900</v>
@@ -29869,13 +30450,16 @@
       <c r="BI158" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ158" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="159" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>177</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E159" s="5">
         <v>14900</v>
@@ -30048,16 +30632,19 @@
       <c r="BI159" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ159" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="160" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D160" s="2">
         <v>14900</v>
@@ -30233,13 +30820,16 @@
       <c r="BI160" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ160" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="161" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>179</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E161" s="5">
         <v>14900</v>
@@ -30412,13 +31002,16 @@
       <c r="BI161" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ161" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="162" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D162" s="2">
         <v>14900</v>
@@ -30594,16 +31187,19 @@
       <c r="BI162" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ162" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="163" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E163" s="5">
         <v>14900</v>
@@ -30776,16 +31372,19 @@
       <c r="BI163" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ163" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="164" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="164" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D164" s="2">
         <v>14900</v>
@@ -30961,13 +31560,16 @@
       <c r="BI164" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ164" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="165" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="165" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>183</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E165" s="5">
         <v>14900</v>
@@ -31140,13 +31742,16 @@
       <c r="BI165" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ165" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="166" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="166" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D166" s="2">
         <v>14900</v>
@@ -31322,13 +31927,16 @@
       <c r="BI166" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ166" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="167" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="167" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>185</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E167" s="5">
         <v>14900</v>
@@ -31501,13 +32109,16 @@
       <c r="BI167" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ167" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="168" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="168" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>186</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D168" s="2">
         <v>14900</v>
@@ -31683,13 +32294,16 @@
       <c r="BI168" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ168" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="169" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="169" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>187</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E169" s="5">
         <v>14900</v>
@@ -31862,13 +32476,16 @@
       <c r="BI169" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ169" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="170" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="170" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>188</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D170" s="2">
         <v>14900</v>
@@ -32044,13 +32661,16 @@
       <c r="BI170" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ170" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="171" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="171" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>189</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E171" s="5">
         <v>14900</v>
@@ -32223,13 +32843,16 @@
       <c r="BI171" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ171" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="172" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="172" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>190</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D172" s="2">
         <v>14900</v>
@@ -32405,13 +33028,16 @@
       <c r="BI172" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ172" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="173" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="173" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>191</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E173" s="5">
         <v>14900</v>
@@ -32584,13 +33210,16 @@
       <c r="BI173" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ173" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="174" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="174" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>192</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D174" s="2">
         <v>14900</v>
@@ -32766,13 +33395,16 @@
       <c r="BI174" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ174" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="175" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="175" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>193</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E175" s="5">
         <v>14900</v>
@@ -32945,13 +33577,16 @@
       <c r="BI175" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ175" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="176" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="176" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>194</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E176" s="5">
         <v>14900</v>
@@ -33124,13 +33759,16 @@
       <c r="BI176" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ176" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="177" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="177" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>195</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E177" s="5">
         <v>60000</v>
@@ -33303,13 +33941,16 @@
       <c r="BI177" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ177" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="178" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="178" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>196</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E178" s="5">
         <v>14900</v>
@@ -33482,13 +34123,16 @@
       <c r="BI178" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ178" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="179" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="179" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E179" s="5">
         <v>52106</v>
@@ -33661,13 +34305,16 @@
       <c r="BI179" s="2">
         <v>60106</v>
       </c>
+      <c r="BJ179" s="2">
+        <v>60106</v>
+      </c>
     </row>
-    <row r="180" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="180" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>198</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E180" s="5">
         <v>14900</v>
@@ -33840,13 +34487,16 @@
       <c r="BI180" s="2">
         <v>14900</v>
       </c>
+      <c r="BJ180" s="2">
+        <v>14900</v>
+      </c>
     </row>
-    <row r="181" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="181" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>199</v>
+        <v>225</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E181" s="5">
         <v>52106</v>
@@ -34019,13 +34669,16 @@
       <c r="BI181" s="2">
         <v>60106</v>
       </c>
+      <c r="BJ181" s="2">
+        <v>60106</v>
+      </c>
     </row>
-    <row r="182" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="182" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E182" s="5">
         <v>52000</v>
@@ -34198,13 +34851,16 @@
       <c r="BI182" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ182" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="183" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="183" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E183" s="5">
         <v>52000</v>
@@ -34377,13 +35033,16 @@
       <c r="BI183" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ183" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="184" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="184" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E184" s="5">
         <v>52000</v>
@@ -34556,13 +35215,16 @@
       <c r="BI184" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ184" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="185" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="185" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E185" s="5">
         <v>63999</v>
@@ -34576,172 +35238,175 @@
       <c r="H185" s="5">
         <v>63999</v>
       </c>
-      <c r="I185" s="5">
+      <c r="I185" s="2">
         <v>63999</v>
       </c>
-      <c r="J185" s="5">
+      <c r="J185" s="2">
         <v>63999</v>
       </c>
-      <c r="K185" s="5">
+      <c r="K185" s="2">
         <v>63999</v>
       </c>
-      <c r="L185" s="5">
+      <c r="L185" s="2">
         <v>63999</v>
       </c>
-      <c r="M185" s="5">
+      <c r="M185" s="2">
         <v>63999</v>
       </c>
-      <c r="N185" s="5">
+      <c r="N185" s="2">
         <v>63999</v>
       </c>
-      <c r="O185" s="5">
+      <c r="O185" s="2">
         <v>63999</v>
       </c>
-      <c r="P185" s="5">
+      <c r="P185" s="2">
         <v>63999</v>
       </c>
-      <c r="Q185" s="5">
+      <c r="Q185" s="2">
         <v>63999</v>
       </c>
-      <c r="R185" s="5">
+      <c r="R185" s="2">
         <v>63999</v>
       </c>
-      <c r="S185" s="5">
+      <c r="S185" s="2">
         <v>63999</v>
       </c>
-      <c r="T185" s="5">
+      <c r="T185" s="2">
         <v>63999</v>
       </c>
-      <c r="U185" s="5">
+      <c r="U185" s="2">
         <v>63999</v>
       </c>
-      <c r="V185" s="5">
+      <c r="V185" s="2">
         <v>63999</v>
       </c>
-      <c r="W185" s="5">
+      <c r="W185" s="2">
         <v>63999</v>
       </c>
-      <c r="X185" s="5">
+      <c r="X185" s="2">
         <v>63999</v>
       </c>
-      <c r="Y185" s="5">
+      <c r="Y185" s="2">
         <v>63999</v>
       </c>
-      <c r="Z185" s="5">
+      <c r="Z185" s="2">
         <v>63999</v>
       </c>
-      <c r="AA185" s="5">
+      <c r="AA185" s="2">
         <v>63999</v>
       </c>
-      <c r="AB185" s="5">
+      <c r="AB185" s="2">
         <v>63999</v>
       </c>
-      <c r="AC185" s="5">
+      <c r="AC185" s="2">
         <v>63999</v>
       </c>
-      <c r="AD185" s="5">
+      <c r="AD185" s="2">
         <v>63999</v>
       </c>
-      <c r="AE185" s="5">
+      <c r="AE185" s="2">
         <v>63999</v>
       </c>
-      <c r="AF185" s="5">
+      <c r="AF185" s="2">
         <v>63999</v>
       </c>
-      <c r="AG185" s="5">
+      <c r="AG185" s="2">
         <v>63999</v>
       </c>
-      <c r="AH185" s="5">
+      <c r="AH185" s="2">
         <v>63999</v>
       </c>
-      <c r="AI185" s="5">
+      <c r="AI185" s="2">
         <v>63999</v>
       </c>
-      <c r="AJ185" s="5">
+      <c r="AJ185" s="2">
         <v>63999</v>
       </c>
-      <c r="AK185" s="5">
+      <c r="AK185" s="2">
         <v>63999</v>
       </c>
-      <c r="AL185" s="5">
+      <c r="AL185" s="2">
         <v>63999</v>
       </c>
-      <c r="AM185" s="5">
+      <c r="AM185" s="2">
         <v>63999</v>
       </c>
-      <c r="AN185" s="5">
+      <c r="AN185" s="2">
         <v>63999</v>
       </c>
-      <c r="AO185" s="5">
+      <c r="AO185" s="2">
         <v>63999</v>
       </c>
-      <c r="AP185" s="5">
+      <c r="AP185" s="2">
         <v>63999</v>
       </c>
-      <c r="AQ185" s="5">
+      <c r="AQ185" s="2">
         <v>63999</v>
       </c>
-      <c r="AR185" s="5">
+      <c r="AR185" s="2">
         <v>63999</v>
       </c>
-      <c r="AS185" s="5">
+      <c r="AS185" s="2">
         <v>63999</v>
       </c>
-      <c r="AT185" s="5">
+      <c r="AT185" s="2">
         <v>63999</v>
       </c>
-      <c r="AU185" s="5">
+      <c r="AU185" s="2">
         <v>63999</v>
       </c>
-      <c r="AV185" s="5">
+      <c r="AV185" s="2">
         <v>63999</v>
       </c>
-      <c r="AW185" s="5">
+      <c r="AW185" s="2">
         <v>63999</v>
       </c>
-      <c r="AX185" s="5">
+      <c r="AX185" s="2">
         <v>63999</v>
       </c>
-      <c r="AY185" s="5">
+      <c r="AY185" s="2">
         <v>63999</v>
       </c>
-      <c r="AZ185" s="5">
+      <c r="AZ185" s="2">
         <v>63999</v>
       </c>
-      <c r="BA185" s="5">
+      <c r="BA185" s="2">
         <v>63999</v>
       </c>
-      <c r="BB185" s="5">
+      <c r="BB185" s="2">
         <v>63999</v>
       </c>
-      <c r="BC185" s="5">
+      <c r="BC185" s="2">
         <v>63999</v>
       </c>
-      <c r="BD185" s="5">
+      <c r="BD185" s="2">
         <v>63999</v>
       </c>
-      <c r="BE185" s="5">
+      <c r="BE185" s="2">
         <v>63999</v>
       </c>
-      <c r="BF185" s="5">
+      <c r="BF185" s="2">
         <v>63999</v>
       </c>
-      <c r="BG185" s="5">
+      <c r="BG185" s="2">
         <v>63999</v>
       </c>
-      <c r="BH185" s="5">
+      <c r="BH185" s="2">
         <v>63999</v>
       </c>
-      <c r="BI185" s="5">
+      <c r="BI185" s="2">
         <v>63999</v>
       </c>
+      <c r="BJ185" s="2">
+        <v>63999</v>
+      </c>
     </row>
-    <row r="186" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="186" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D186" s="2">
         <v>14900</v>
@@ -34917,78 +35582,31 @@
       <c r="BI186" s="2">
         <v>60200</v>
       </c>
+      <c r="BJ186" s="2">
+        <v>60200</v>
+      </c>
     </row>
-    <row r="187" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="187" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E187" s="5"/>
       <c r="F187" s="5"/>
       <c r="G187" s="5"/>
       <c r="H187" s="5"/>
-      <c r="I187" s="5"/>
-      <c r="J187" s="5"/>
-      <c r="K187" s="5"/>
-      <c r="L187" s="5"/>
-      <c r="M187" s="5"/>
-      <c r="N187" s="5"/>
-      <c r="O187" s="5"/>
-      <c r="P187" s="5"/>
-      <c r="Q187" s="5"/>
-      <c r="R187" s="5"/>
-      <c r="S187" s="5"/>
-      <c r="T187" s="5"/>
-      <c r="U187" s="5"/>
-      <c r="V187" s="5"/>
-      <c r="W187" s="5"/>
-      <c r="X187" s="5"/>
-      <c r="Y187" s="5"/>
-      <c r="Z187" s="5"/>
-      <c r="AA187" s="5"/>
-      <c r="AB187" s="5"/>
-      <c r="AC187" s="5"/>
-      <c r="AD187" s="5"/>
-      <c r="AE187" s="5"/>
-      <c r="AF187" s="5"/>
-      <c r="AG187" s="5"/>
-      <c r="AH187" s="5"/>
-      <c r="AI187" s="5"/>
-      <c r="AJ187" s="5"/>
-      <c r="AK187" s="5"/>
-      <c r="AL187" s="5"/>
-      <c r="AM187" s="5"/>
-      <c r="AN187" s="5"/>
-      <c r="AO187" s="5"/>
-      <c r="AP187" s="5"/>
-      <c r="AQ187" s="5"/>
-      <c r="AR187" s="5"/>
-      <c r="AS187" s="5"/>
-      <c r="AT187" s="5"/>
-      <c r="AU187" s="5"/>
-      <c r="AV187" s="5"/>
-      <c r="AW187" s="5"/>
-      <c r="AX187" s="5"/>
-      <c r="AY187" s="5"/>
-      <c r="AZ187" s="5"/>
-      <c r="BA187" s="5"/>
-      <c r="BB187" s="5"/>
-      <c r="BC187" s="5"/>
-      <c r="BD187" s="5"/>
-      <c r="BE187" s="5"/>
-      <c r="BF187" s="5"/>
-      <c r="BG187" s="5"/>
-      <c r="BH187" s="5"/>
-      <c r="BI187" s="5"/>
+      <c r="BD187" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="188" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="188" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E188" s="5">
         <v>52000</v>
@@ -35161,13 +35779,16 @@
       <c r="BI188" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ188" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="189" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="189" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E189" s="5">
         <v>52000</v>
@@ -35340,13 +35961,16 @@
       <c r="BI189" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ189" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="190" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="190" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E190" s="5">
         <v>52000</v>
@@ -35519,13 +36143,16 @@
       <c r="BI190" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ190" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="191" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="191" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E191" s="5">
         <v>53005</v>
@@ -35698,13 +36325,16 @@
       <c r="BI191" s="2">
         <v>53005</v>
       </c>
+      <c r="BJ191" s="2">
+        <v>53005</v>
+      </c>
     </row>
-    <row r="192" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="192" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E192" s="5">
         <v>52000</v>
@@ -35877,13 +36507,16 @@
       <c r="BI192" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ192" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="193" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="193" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E193" s="5">
         <v>52000</v>
@@ -36056,13 +36689,16 @@
       <c r="BI193" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ193" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="194" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="194" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E194" s="5">
         <v>52100</v>
@@ -36235,13 +36871,16 @@
       <c r="BI194" s="2">
         <v>60100</v>
       </c>
+      <c r="BJ194" s="2">
+        <v>60100</v>
+      </c>
     </row>
-    <row r="195" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="195" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E195" s="5">
         <v>52000</v>
@@ -36414,134 +37053,137 @@
       <c r="BI195" s="2">
         <v>60000</v>
       </c>
+      <c r="BJ195" s="2">
+        <v>60000</v>
+      </c>
     </row>
-    <row r="196" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="196" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B196" s="6"/>
       <c r="C196" s="8"/>
     </row>
-    <row r="197" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="197" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
         <v>144</v>
       </c>
       <c r="B197" s="6"/>
       <c r="C197" s="8"/>
     </row>
-    <row r="198" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="198" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B198" s="6"/>
       <c r="C198" s="8"/>
     </row>
-    <row r="199" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="199" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
         <v>146</v>
       </c>
       <c r="B199" s="6"/>
       <c r="C199" s="8"/>
     </row>
-    <row r="200" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="200" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
         <v>147</v>
       </c>
       <c r="B200" s="6"/>
       <c r="C200" s="8"/>
     </row>
-    <row r="201" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="201" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B201" s="6"/>
       <c r="C201" s="8"/>
     </row>
-    <row r="202" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="202" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
         <v>149</v>
       </c>
       <c r="B202" s="6"/>
       <c r="C202" s="8"/>
     </row>
-    <row r="203" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="203" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
         <v>150</v>
       </c>
       <c r="B203" s="6"/>
       <c r="C203" s="8"/>
     </row>
-    <row r="204" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="204" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A204" s="7" t="s">
         <v>151</v>
       </c>
       <c r="B204" s="6"/>
       <c r="C204" s="8"/>
     </row>
-    <row r="205" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="205" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
         <v>152</v>
       </c>
       <c r="B205" s="6"/>
       <c r="C205" s="8"/>
     </row>
-    <row r="206" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="206" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A206" s="7" t="s">
         <v>153</v>
       </c>
       <c r="B206" s="6"/>
       <c r="C206" s="8"/>
     </row>
-    <row r="207" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="207" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A207" s="7" t="s">
         <v>154</v>
       </c>
       <c r="B207" s="6"/>
       <c r="C207" s="8"/>
     </row>
-    <row r="208" spans="1:61" x14ac:dyDescent="0.75">
+    <row r="208" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
         <v>155</v>
       </c>
       <c r="B208" s="6"/>
       <c r="C208" s="8"/>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="7" t="s">
         <v>156</v>
       </c>
       <c r="B209" s="6"/>
       <c r="C209" s="8"/>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="7" t="s">
         <v>157</v>
       </c>
       <c r="B210" s="6"/>
       <c r="C210" s="8"/>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="9" t="s">
         <v>158</v>
       </c>
       <c r="B211" s="6"/>
       <c r="C211" s="8"/>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="9" t="s">
         <v>159</v>
       </c>
       <c r="B212" s="6"/>
       <c r="C212" s="8"/>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
         <v>160</v>
       </c>
       <c r="B213" s="6"/>
       <c r="C213" s="8"/>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
         <v>161</v>
       </c>
@@ -36549,8 +37191,23 @@
       <c r="C214" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BI195" xr:uid="{564C415C-277C-4055-8EB4-768220830CF2}"/>
+  <autoFilter ref="A1:BJ214" xr:uid="{564C415C-277C-4055-8EB4-768220830CF2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D457A691-92EF-4DDB-B234-A26954DF1BC8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>